<commit_message>
updated with iowa results
</commit_message>
<xml_diff>
--- a/public/data/wikipedia_county_level_election_results.xlsx
+++ b/public/data/wikipedia_county_level_election_results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afmcgovern\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="5010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Alabama</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/United_States_presidential_election_in_Connecticut,_2016#Results_by_County</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/United_States_presidential_election_in_Georgia,_2016#Results_by_County</t>
   </si>
 </sst>
 </file>
@@ -256,8 +262,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C29" totalsRowShown="0">
-  <autoFilter ref="A1:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C30" totalsRowShown="0">
+  <autoFilter ref="A1:C30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="State"/>
     <tableColumn id="2" name="URL"/>
@@ -566,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -688,240 +694,252 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C10" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Iowa",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Iowa,_2016#By_county"},</v>
+        <v>{ state: "Georgia",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Georgia,_2016#Results_by_County"},</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Kentucky",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Kentucky,_2016#By_county"},</v>
+        <v>{ state: "Iowa",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Iowa,_2016#By_county"},</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Maryland",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Maryland,_2016#By_county"},</v>
+        <v>{ state: "Kentucky",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Kentucky,_2016#By_county"},</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Michigan",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Michigan,_2016#Results_by_county"},</v>
+        <v>{ state: "Maryland",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Maryland,_2016#By_county"},</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Missouri",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Missouri,_2016#Results_by_county.5B9.5D"},</v>
+        <v>{ state: "Michigan",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Michigan,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Montana",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Montana,_2016#Results_by_county"},</v>
+        <v>{ state: "Missouri",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Missouri,_2016#Results_by_county.5B9.5D"},</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Nebraska",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Nebraska,_2016#Results_by_county"},</v>
+        <v>{ state: "Montana",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Montana,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Nevada",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Nevada,_2016#Results_by_county"},</v>
+        <v>{ state: "Nebraska",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Nebraska,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "New Jersey",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_New Jersey,_2016#cite_ref-Official_res_2-2"},</v>
+        <v>{ state: "Nevada",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Nevada,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "New Mexico",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_New Mexico,_2016#Results_by_county"},</v>
+        <v>{ state: "New Jersey",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_New Jersey,_2016#cite_ref-Official_res_2-2"},</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "North Carolina",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_North Carolina,_2016#By_county"},</v>
+        <v>{ state: "New Mexico",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_New Mexico,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Ohio",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Ohio,_2016#By_county"},</v>
+        <v>{ state: "North Carolina",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_North Carolina,_2016#By_county"},</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Oklahoma",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Oklahoma,_2016#Results_by_County"},</v>
+        <v>{ state: "Ohio",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Ohio,_2016#By_county"},</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Oregon",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Oregon,_2016#Results_by_county"},</v>
+        <v>{ state: "Oklahoma",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Oklahoma,_2016#Results_by_County"},</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Rhode Island",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Rhode Island,_2016#Results_by_county"},</v>
+        <v>{ state: "Oregon",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Oregon,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "South Dakota",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_South Dakota,_2016#Results_by_county"},</v>
+        <v>{ state: "Rhode Island",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Rhode Island,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Texas",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Texas,_2016#By_county"},</v>
+        <v>{ state: "South Dakota",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_South Dakota,_2016#Results_by_county"},</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Utah",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Utah,_2016#By_county"},</v>
+        <v>{ state: "Texas",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Texas,_2016#By_county"},</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
-        <v>{ state: "Washington",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Washington,_2016#By_county"},</v>
+        <v>{ state: "Utah",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Utah,_2016#By_county"},</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="str">
+        <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
+        <v>{ state: "Washington",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Washington,_2016#By_county"},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>52</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>53</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C30" t="str">
         <f>"{ state: "&amp;CHAR(34)&amp;Table1[[#This Row],[State]]&amp;CHAR(34)&amp;",URL: "&amp;CHAR(34)&amp;Table1[[#This Row],[URL]]&amp;CHAR(34)&amp;"},"</f>
         <v>{ state: "Wisconsin",URL: "https://en.wikipedia.org/wiki/United_States_presidential_election_in_Wisconsin,_2016#Results_by_county"},</v>
       </c>

</xml_diff>